<commit_message>
ng: add oncho adamawa forms.
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Nigeria/2024/adamawa/ng_oncho_stop_202403_1_site_adam.xlsx
+++ b/ONCHO/Impact Assessments/Nigeria/2024/adamawa/ng_oncho_stop_202403_1_site_adam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Nigeria\2024\ogun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Nigeria\2024\adamawa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349068A4-EC6A-4ED8-8A2A-9C4F369C3717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A77393-3E1B-41BA-8EEE-1B5173B68DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="156">
   <si>
     <t>type</t>
   </si>
@@ -383,118 +383,124 @@
     <t>English</t>
   </si>
   <si>
-    <t>ng_oncho_stop_202403_1_site_ogun</t>
-  </si>
-  <si>
-    <t>(2024 Mar) - 1. Site Form - Ogun State</t>
-  </si>
-  <si>
-    <t>OGUN</t>
-  </si>
-  <si>
-    <t>ABEOKUTA NORTH</t>
-  </si>
-  <si>
-    <t>ADO ODO/OTA</t>
-  </si>
-  <si>
-    <t>ADO-ODO/OTA (BADAGRY)</t>
-  </si>
-  <si>
-    <t>EGBADO NORTH</t>
-  </si>
-  <si>
-    <t>IFO</t>
-  </si>
-  <si>
-    <t>IJEBU EAST</t>
-  </si>
-  <si>
-    <t>IJEBU NORTH</t>
-  </si>
-  <si>
-    <t>IJEBU-ODE</t>
-  </si>
-  <si>
-    <t>IMEKO AFON</t>
-  </si>
-  <si>
-    <t>OBAFEMI O</t>
-  </si>
-  <si>
-    <t>OBAFEMI OWODE</t>
-  </si>
-  <si>
-    <t>ODEDA</t>
-  </si>
-  <si>
-    <t>ODOGBOLU</t>
-  </si>
-  <si>
-    <t>SAGAMU</t>
-  </si>
-  <si>
-    <t>YEWA SOUTH</t>
-  </si>
-  <si>
-    <t>ATAPA IKOYI</t>
-  </si>
-  <si>
-    <t>IDIMU</t>
-  </si>
-  <si>
-    <t>SEJE</t>
-  </si>
-  <si>
-    <t>EGGUA</t>
-  </si>
-  <si>
-    <t>SAALA-ORILE</t>
-  </si>
-  <si>
-    <t>ASANI</t>
-  </si>
-  <si>
-    <t>OKE-MAKUN</t>
-  </si>
-  <si>
-    <t>AJEGUNLE AWA</t>
-  </si>
-  <si>
-    <t>DAMOLA</t>
-  </si>
-  <si>
-    <t>MOSINMI</t>
-  </si>
-  <si>
-    <t>IRAWO</t>
-  </si>
-  <si>
-    <t>ALLA SOKA</t>
-  </si>
-  <si>
-    <t>IDOFA</t>
-  </si>
-  <si>
-    <t>AROGUN</t>
-  </si>
-  <si>
-    <t>OLOJO</t>
-  </si>
-  <si>
-    <t>ABULE SET</t>
-  </si>
-  <si>
-    <t>JAGUNA</t>
-  </si>
-  <si>
-    <t>OKUN-OWO</t>
-  </si>
-  <si>
-    <t>ODELEMO</t>
-  </si>
-  <si>
-    <t>IDOGO</t>
+    <t>ng_oncho_stop_202403_1_site_adam</t>
+  </si>
+  <si>
+    <t>(Adamawa State 2024 Apr) - 1. Site Form</t>
+  </si>
+  <si>
+    <t>ADAMAWA</t>
+  </si>
+  <si>
+    <t>DEMSA</t>
+  </si>
+  <si>
+    <t>FUFORE</t>
+  </si>
+  <si>
+    <t>GIRIE</t>
+  </si>
+  <si>
+    <t>GOMBI</t>
+  </si>
+  <si>
+    <t>GUYUK</t>
+  </si>
+  <si>
+    <t>HONG</t>
+  </si>
+  <si>
+    <t>JADA</t>
+  </si>
+  <si>
+    <t>LAMURDE</t>
+  </si>
+  <si>
+    <t>MADAGALI</t>
+  </si>
+  <si>
+    <t>MICHIKA</t>
+  </si>
+  <si>
+    <t>MUBI NORTH</t>
+  </si>
+  <si>
+    <t>MUBI SOUTH</t>
+  </si>
+  <si>
+    <t>SONG</t>
+  </si>
+  <si>
+    <t>TEUNGO</t>
+  </si>
+  <si>
+    <t>YOLA NORTH</t>
+  </si>
+  <si>
+    <t>BARWO</t>
+  </si>
+  <si>
+    <t>BIRIJI</t>
+  </si>
+  <si>
+    <t>BOLANGA</t>
+  </si>
+  <si>
+    <t>BOLLERE</t>
+  </si>
+  <si>
+    <t>DABEWA</t>
+  </si>
+  <si>
+    <t>DAMAI</t>
+  </si>
+  <si>
+    <t>DELHI</t>
+  </si>
+  <si>
+    <t>DESEL</t>
+  </si>
+  <si>
+    <t>FALAHI</t>
+  </si>
+  <si>
+    <t>GUYAKU</t>
+  </si>
+  <si>
+    <t>HEATIYI</t>
+  </si>
+  <si>
+    <t>JAMTARI</t>
+  </si>
+  <si>
+    <t>KOCCIEL</t>
+  </si>
+  <si>
+    <t>KOMBOR</t>
+  </si>
+  <si>
+    <t>KWATAMA DAFFA</t>
+  </si>
+  <si>
+    <t>MUCHALLA</t>
+  </si>
+  <si>
+    <t>PUBA</t>
+  </si>
+  <si>
+    <t>SINA MALA</t>
+  </si>
+  <si>
+    <t>TUNGO</t>
+  </si>
+  <si>
+    <t>WURO HAMMAGU</t>
+  </si>
+  <si>
+    <t>WURO JATAU</t>
+  </si>
+  <si>
+    <t>YOLA</t>
   </si>
 </sst>
 </file>
@@ -944,7 +950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -1412,11 +1418,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD81"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87:A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1425,6 +1431,7 @@
     <col min="2" max="2" width="39.625" customWidth="1"/>
     <col min="3" max="3" width="23.75" customWidth="1"/>
     <col min="4" max="4" width="11.75" customWidth="1"/>
+    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1936,7 +1943,7 @@
         <v>134</v>
       </c>
       <c r="E41" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1950,7 +1957,7 @@
         <v>135</v>
       </c>
       <c r="E42" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1964,7 +1971,7 @@
         <v>136</v>
       </c>
       <c r="E43" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1978,7 +1985,7 @@
         <v>137</v>
       </c>
       <c r="E44" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1992,7 +1999,7 @@
         <v>138</v>
       </c>
       <c r="E45" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2006,7 +2013,7 @@
         <v>139</v>
       </c>
       <c r="E46" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2020,7 +2027,7 @@
         <v>140</v>
       </c>
       <c r="E47" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2028,265 +2035,265 @@
         <v>89</v>
       </c>
       <c r="B48" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="C48" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E48" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>89</v>
       </c>
       <c r="B49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E49" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E50" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>89</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E51" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>89</v>
       </c>
       <c r="B52" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C52" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E52" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>89</v>
       </c>
       <c r="B53" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="C53" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E53" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>89</v>
       </c>
       <c r="B54" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C54" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E54" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>89</v>
       </c>
       <c r="B55" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C55" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E55" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>89</v>
       </c>
       <c r="B56" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C56" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E56" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>89</v>
       </c>
       <c r="B57" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C57" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E57" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>89</v>
       </c>
       <c r="B58" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="C58" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="E58" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>89</v>
       </c>
       <c r="B59" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C59" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E59" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>89</v>
       </c>
       <c r="B60" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" t="s">
+        <v>150</v>
+      </c>
+      <c r="E60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61" t="s">
+        <v>151</v>
+      </c>
+      <c r="E61" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62" t="s">
+        <v>132</v>
+      </c>
+      <c r="E62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" t="s">
+        <v>152</v>
+      </c>
+      <c r="E63" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>89</v>
+      </c>
+      <c r="B64" t="s">
         <v>153</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C64" t="s">
         <v>153</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E64" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>89</v>
+      </c>
+      <c r="B65" t="s">
+        <v>154</v>
+      </c>
+      <c r="C65" t="s">
+        <v>154</v>
+      </c>
+      <c r="E65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" t="s">
+        <v>155</v>
+      </c>
+      <c r="C66" t="s">
+        <v>155</v>
+      </c>
+      <c r="E66" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B62">
-        <v>201</v>
-      </c>
-      <c r="C62">
-        <v>201</v>
-      </c>
-      <c r="F62" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B63">
-        <v>202</v>
-      </c>
-      <c r="C63">
-        <v>202</v>
-      </c>
-      <c r="F63" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B64">
-        <v>203</v>
-      </c>
-      <c r="C64">
-        <v>203</v>
-      </c>
-      <c r="F64" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B65">
-        <v>204</v>
-      </c>
-      <c r="C65">
-        <v>204</v>
-      </c>
-      <c r="F65" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B66">
-        <v>205</v>
-      </c>
-      <c r="C66">
-        <v>205</v>
-      </c>
-      <c r="F66" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B67">
-        <v>206</v>
-      </c>
-      <c r="C67">
-        <v>206</v>
-      </c>
-      <c r="F67" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2294,13 +2301,13 @@
         <v>111</v>
       </c>
       <c r="B68">
-        <v>207</v>
+        <v>301</v>
       </c>
       <c r="C68">
-        <v>207</v>
+        <v>301</v>
       </c>
       <c r="F68" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2308,13 +2315,13 @@
         <v>111</v>
       </c>
       <c r="B69">
-        <v>208</v>
+        <v>302</v>
       </c>
       <c r="C69">
-        <v>208</v>
+        <v>302</v>
       </c>
       <c r="F69" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2322,13 +2329,13 @@
         <v>111</v>
       </c>
       <c r="B70">
-        <v>209</v>
+        <v>303</v>
       </c>
       <c r="C70">
-        <v>209</v>
+        <v>303</v>
       </c>
       <c r="F70" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2336,13 +2343,13 @@
         <v>111</v>
       </c>
       <c r="B71">
-        <v>210</v>
+        <v>304</v>
       </c>
       <c r="C71">
-        <v>210</v>
+        <v>304</v>
       </c>
       <c r="F71" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2350,13 +2357,13 @@
         <v>111</v>
       </c>
       <c r="B72">
-        <v>211</v>
+        <v>305</v>
       </c>
       <c r="C72">
-        <v>211</v>
+        <v>305</v>
       </c>
       <c r="F72" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2364,13 +2371,13 @@
         <v>111</v>
       </c>
       <c r="B73">
-        <v>212</v>
+        <v>306</v>
       </c>
       <c r="C73">
-        <v>212</v>
+        <v>306</v>
       </c>
       <c r="F73" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2378,13 +2385,13 @@
         <v>111</v>
       </c>
       <c r="B74">
-        <v>213</v>
+        <v>307</v>
       </c>
       <c r="C74">
-        <v>213</v>
+        <v>307</v>
       </c>
       <c r="F74" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2392,13 +2399,13 @@
         <v>111</v>
       </c>
       <c r="B75">
-        <v>214</v>
+        <v>308</v>
       </c>
       <c r="C75">
-        <v>214</v>
+        <v>308</v>
       </c>
       <c r="F75" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2406,10 +2413,10 @@
         <v>111</v>
       </c>
       <c r="B76">
-        <v>215</v>
+        <v>309</v>
       </c>
       <c r="C76">
-        <v>215</v>
+        <v>309</v>
       </c>
       <c r="F76" t="s">
         <v>148</v>
@@ -2420,13 +2427,13 @@
         <v>111</v>
       </c>
       <c r="B77">
-        <v>216</v>
+        <v>310</v>
       </c>
       <c r="C77">
-        <v>216</v>
+        <v>310</v>
       </c>
       <c r="F77" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2434,13 +2441,13 @@
         <v>111</v>
       </c>
       <c r="B78">
-        <v>217</v>
+        <v>311</v>
       </c>
       <c r="C78">
-        <v>217</v>
+        <v>311</v>
       </c>
       <c r="F78" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2448,13 +2455,13 @@
         <v>111</v>
       </c>
       <c r="B79">
-        <v>218</v>
+        <v>312</v>
       </c>
       <c r="C79">
-        <v>218</v>
+        <v>312</v>
       </c>
       <c r="F79" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2462,13 +2469,13 @@
         <v>111</v>
       </c>
       <c r="B80">
-        <v>219</v>
+        <v>313</v>
       </c>
       <c r="C80">
-        <v>219</v>
+        <v>313</v>
       </c>
       <c r="F80" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2476,13 +2483,209 @@
         <v>111</v>
       </c>
       <c r="B81">
-        <v>220</v>
+        <v>314</v>
       </c>
       <c r="C81">
-        <v>220</v>
+        <v>314</v>
       </c>
       <c r="F81" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B82">
+        <v>315</v>
+      </c>
+      <c r="C82">
+        <v>315</v>
+      </c>
+      <c r="F82" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B83">
+        <v>316</v>
+      </c>
+      <c r="C83">
+        <v>316</v>
+      </c>
+      <c r="F83" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B84">
+        <v>317</v>
+      </c>
+      <c r="C84">
+        <v>317</v>
+      </c>
+      <c r="F84" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B85">
+        <v>318</v>
+      </c>
+      <c r="C85">
+        <v>318</v>
+      </c>
+      <c r="F85" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B86">
+        <v>319</v>
+      </c>
+      <c r="C86">
+        <v>319</v>
+      </c>
+      <c r="F86" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B87">
+        <v>320</v>
+      </c>
+      <c r="C87">
+        <v>320</v>
+      </c>
+      <c r="F87" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B88">
+        <v>321</v>
+      </c>
+      <c r="C88">
+        <v>321</v>
+      </c>
+      <c r="F88" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B89">
+        <v>322</v>
+      </c>
+      <c r="C89">
+        <v>322</v>
+      </c>
+      <c r="F89" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B90">
+        <v>323</v>
+      </c>
+      <c r="C90">
+        <v>323</v>
+      </c>
+      <c r="F90" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B91">
+        <v>324</v>
+      </c>
+      <c r="C91">
+        <v>324</v>
+      </c>
+      <c r="F91" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B92">
+        <v>325</v>
+      </c>
+      <c r="C92">
+        <v>325</v>
+      </c>
+      <c r="F92" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B93">
+        <v>326</v>
+      </c>
+      <c r="C93">
+        <v>326</v>
+      </c>
+      <c r="F93" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B94">
+        <v>327</v>
+      </c>
+      <c r="C94">
+        <v>327</v>
+      </c>
+      <c r="F94" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B95">
+        <v>328</v>
+      </c>
+      <c r="C95">
+        <v>328</v>
+      </c>
+      <c r="F95" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2499,7 +2702,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>